<commit_message>
[Pipette] Main PCB 수정 - Slide SW 결정 필요
</commit_message>
<xml_diff>
--- a/Plasma_Gen_Device cost.xlsx
+++ b/Plasma_Gen_Device cost.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Transformer" sheetId="1" r:id="rId1"/>
     <sheet name="MOSFET" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Pipette" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="107">
   <si>
     <t>PN</t>
   </si>
@@ -362,6 +363,62 @@
   </si>
   <si>
     <t>2/5일 구매</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>053048-0410</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.25mm Pitch CON,4-Pin, Dip Right angle_Molex</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> P005634295 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>053048-0310</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.25mm Pitch CON,3-Pin, Dip Right angle_Molex</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSS-1300C</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP3T slide Switch, Straight DIP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP3T slide Switch, DIP Right Angle, 3.0x12.5x2.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP3T slide Switch, SMD Right Angle, 3.0x12.5x2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> P000394667 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> P000394663 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSS-1310TB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> P006911086 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSS-1310MC</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -788,7 +845,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1094,6 +1151,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1250,7 +1316,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
@@ -1379,47 +1445,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="53">
     <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1647,7 +1720,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1682,7 +1755,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1893,8 +1966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1944,13 +2017,13 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="79" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -1978,9 +2051,9 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="71"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
       <c r="E5" s="8" t="s">
         <v>16</v>
       </c>
@@ -2066,22 +2139,22 @@
       <c r="K7" s="12"/>
     </row>
     <row r="8" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="70" t="s">
         <v>83</v>
       </c>
       <c r="C8" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="79" t="s">
+      <c r="E8" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="79">
+      <c r="F8" s="72">
         <v>1</v>
       </c>
-      <c r="G8" s="80">
+      <c r="G8" s="73">
         <v>960</v>
       </c>
       <c r="H8" s="22">
@@ -2177,13 +2250,13 @@
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="70" t="s">
+      <c r="C12" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="79" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="31" t="s">
@@ -2208,9 +2281,9 @@
       </c>
     </row>
     <row r="13" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="71"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
       <c r="E13" s="8" t="s">
         <v>15</v>
       </c>
@@ -2233,9 +2306,9 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="71"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
       <c r="E14" s="8" t="s">
         <v>12</v>
       </c>
@@ -2367,13 +2440,13 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="70" t="s">
+      <c r="C20" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="72" t="s">
+      <c r="D20" s="78" t="s">
         <v>41</v>
       </c>
       <c r="E20" s="8" t="s">
@@ -2394,9 +2467,9 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="73"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="72"/>
+      <c r="B21" s="80"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="78"/>
       <c r="E21" s="8" t="s">
         <v>15</v>
       </c>
@@ -2415,13 +2488,13 @@
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="70" t="s">
+      <c r="C22" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="72" t="s">
+      <c r="D22" s="78" t="s">
         <v>40</v>
       </c>
       <c r="E22" s="8" t="s">
@@ -2444,9 +2517,9 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="76"/>
-      <c r="C23" s="75"/>
-      <c r="D23" s="74"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="82"/>
+      <c r="D23" s="81"/>
       <c r="E23" s="10" t="s">
         <v>15</v>
       </c>
@@ -2472,7 +2545,7 @@
       <c r="I24" s="9"/>
     </row>
     <row r="26" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
+      <c r="B26" s="85" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2571,22 +2644,22 @@
       </c>
     </row>
     <row r="30" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="77" t="s">
+      <c r="B30" s="70" t="s">
         <v>85</v>
       </c>
       <c r="C30" s="36">
         <v>2</v>
       </c>
-      <c r="D30" s="78" t="s">
+      <c r="D30" s="71" t="s">
         <v>84</v>
       </c>
-      <c r="E30" s="81" t="s">
+      <c r="E30" s="74" t="s">
         <v>15</v>
       </c>
       <c r="F30" s="36">
         <v>1</v>
       </c>
-      <c r="G30" s="82">
+      <c r="G30" s="75">
         <v>960</v>
       </c>
       <c r="H30" s="22">
@@ -2596,7 +2669,7 @@
         <v>16400</v>
       </c>
       <c r="J30" s="33"/>
-      <c r="K30" s="83" t="s">
+      <c r="K30" s="76" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2830,18 +2903,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B12:B14"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B12:B14"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3270,7 +3343,7 @@
         <f>G6/2</f>
         <v>1.1850000000000001</v>
       </c>
-      <c r="H7" s="84">
+      <c r="H7" s="77">
         <f>SUM(F7:G7)</f>
         <v>3.12</v>
       </c>
@@ -3309,4 +3382,169 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>130</v>
+      </c>
+      <c r="K4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="87" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="87"/>
+      <c r="D7" s="86" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>1900</v>
+      </c>
+      <c r="G7">
+        <v>450</v>
+      </c>
+      <c r="K7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="87"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>790</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>700</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Pipette] SCH, PCB 작업 update
</commit_message>
<xml_diff>
--- a/Plasma_Gen_Device cost.xlsx
+++ b/Plasma_Gen_Device cost.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Transformer" sheetId="1" r:id="rId1"/>
-    <sheet name="MOSFET" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="MOSFET" sheetId="2" r:id="rId3"/>
     <sheet name="Pipette" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="155">
   <si>
     <t>PN</t>
   </si>
@@ -390,18 +390,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>SP3T slide Switch, Straight DIP</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SP3T slide Switch, DIP Right Angle, 3.0x12.5x2.0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SP3T slide Switch, SMD Right Angle, 3.0x12.5x2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> P000394667 </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -419,6 +407,206 @@
   </si>
   <si>
     <t>CSS-1310MC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDS5050TCU-S-AP-A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> (주)디웰전자 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>P002343866</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0x5.0x1.6 size, RGB full coler, SMD파워 3색 LED </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lite-On Inc</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>P008219901</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASMT-YTD2-0BB02</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avago</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">P000725384 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LTST-C19HE1WT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">LTST-C19FD1WT </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">P001586603 </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED RGB DIFFUSED 0606 SMD - 0.35T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LED OGB DIFFUSED 0608 SMD - 0.55T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3 color type LED 6-pin, TOP View, R745mcd, G1600mcd, B380mcd</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.4x2.8</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.00mm</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>LTSN-N213EGBW</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lite-On Inc</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.0x12.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.5x12</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.5mm</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CL-SB-13A-1x</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CL-SB-13B-11T</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>P006914254</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CL-SB-13C-11</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>P006913975</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP3T slide Switch, SMD Right Angle, key 2x0.6</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP3T slide Switch, SMD Right Angle, key 2x1.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP3T slide Switch, DIP Right Angle, key 2x1.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP3T slide Switch, DIP Right Angle, key 2x0.6</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP3T slide Switch, Straight DIP, key 2x0.6</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CMS-2314A</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP3T slide Switch, SMD J-hook Right Angle, key 4x1.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SP3T slide Switch, SMD J-hook Right Angle, key 2x1.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nidec Copal Electronics Corporation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nidec Copal Electronics Corporation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4x15</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_size</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>12512WS-02B</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>YEONHO</t>
+  </si>
+  <si>
+    <t>CON 2-pin, Throgh hole  type</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.0x3.6</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2mm</t>
+  </si>
+  <si>
+    <t>053048-0210</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.25mm Pitch CON,2-Pin, Dip Right angle_Molex</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.25x5.5</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status LED</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slide Key</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GAS CON</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -430,7 +618,7 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -644,6 +832,13 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="36">
@@ -1316,7 +1511,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
@@ -1465,12 +1660,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1483,15 +1682,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="53">
@@ -1720,7 +1949,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1755,7 +1984,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2017,7 +2246,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="80" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="79" t="s">
@@ -2051,7 +2280,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="84"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="79"/>
       <c r="D5" s="79"/>
       <c r="E5" s="8" t="s">
@@ -2250,7 +2479,7 @@
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="80" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="79" t="s">
@@ -2281,7 +2510,7 @@
       </c>
     </row>
     <row r="13" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="84"/>
+      <c r="B13" s="80"/>
       <c r="C13" s="79"/>
       <c r="D13" s="79"/>
       <c r="E13" s="8" t="s">
@@ -2306,7 +2535,7 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="84"/>
+      <c r="B14" s="80"/>
       <c r="C14" s="79"/>
       <c r="D14" s="79"/>
       <c r="E14" s="8" t="s">
@@ -2440,13 +2669,13 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="82" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="78" t="s">
+      <c r="D20" s="81" t="s">
         <v>41</v>
       </c>
       <c r="E20" s="8" t="s">
@@ -2467,9 +2696,9 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="80"/>
+      <c r="B21" s="82"/>
       <c r="C21" s="79"/>
-      <c r="D21" s="78"/>
+      <c r="D21" s="81"/>
       <c r="E21" s="8" t="s">
         <v>15</v>
       </c>
@@ -2488,13 +2717,13 @@
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="82" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="78" t="s">
+      <c r="D22" s="81" t="s">
         <v>40</v>
       </c>
       <c r="E22" s="8" t="s">
@@ -2517,9 +2746,9 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="83"/>
-      <c r="C23" s="82"/>
-      <c r="D23" s="81"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="83"/>
       <c r="E23" s="10" t="s">
         <v>15</v>
       </c>
@@ -2545,7 +2774,7 @@
       <c r="I24" s="9"/>
     </row>
     <row r="26" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="85" t="s">
+      <c r="B26" s="78" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2903,18 +3132,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="B12:B14"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B22:B23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2923,6 +3152,88 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C6:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="D6">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F6">
+        <v>3.87</v>
+      </c>
+      <c r="G6">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <f>C6/2</f>
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="D7" s="1">
+        <f>D6/2</f>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="F7" s="1">
+        <f>F6/2</f>
+        <v>1.9350000000000001</v>
+      </c>
+      <c r="G7" s="1">
+        <f>G6/2</f>
+        <v>1.1850000000000001</v>
+      </c>
+      <c r="H7" s="77">
+        <f>SUM(F7:G7)</f>
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F10" s="1">
+        <v>2.4300000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F11" s="1">
+        <f>F10/2</f>
+        <v>1.2150000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>7.6</v>
+      </c>
+      <c r="D14">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="1">
+        <f>C14/2</f>
+        <v>3.8</v>
+      </c>
+      <c r="D15" s="1">
+        <f>D14/2</f>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P37"/>
   <sheetViews>
@@ -3302,105 +3613,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C6">
-        <v>9.1199999999999992</v>
-      </c>
-      <c r="D6">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="F6">
-        <v>3.87</v>
-      </c>
-      <c r="G6">
-        <v>2.37</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C7">
-        <f>C6/2</f>
-        <v>4.5599999999999996</v>
-      </c>
-      <c r="D7" s="1">
-        <f>D6/2</f>
-        <v>2.5499999999999998</v>
-      </c>
-      <c r="F7" s="1">
-        <f>F6/2</f>
-        <v>1.9350000000000001</v>
-      </c>
-      <c r="G7" s="1">
-        <f>G6/2</f>
-        <v>1.1850000000000001</v>
-      </c>
-      <c r="H7" s="77">
-        <f>SUM(F7:G7)</f>
-        <v>3.12</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F10" s="1">
-        <v>2.4300000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F11" s="1">
-        <f>F10/2</f>
-        <v>1.2150000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C14">
-        <v>7.6</v>
-      </c>
-      <c r="D14">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="1">
-        <f>C14/2</f>
-        <v>3.8</v>
-      </c>
-      <c r="D15" s="1">
-        <f>D14/2</f>
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K10"/>
+  <dimension ref="A2:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
@@ -3410,29 +3640,35 @@
       <c r="D3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="95" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" s="95" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="H3" s="14" t="s">
         <v>9</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>31</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>10</v>
       </c>
       <c r="J3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="M3" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>93</v>
       </c>
@@ -3442,100 +3678,391 @@
       <c r="D4" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="48" t="s">
+      <c r="F4" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>10</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>130</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>96</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="F5" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>10</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="87" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="86" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="C7" s="86" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="87" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>1900</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>450</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>790</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="87"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="48" t="s">
+      <c r="C9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="1">
+      <c r="H9" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="1">
-        <v>790</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="I9" s="1">
         <v>700</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="M9" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="D10" s="1" t="s">
-        <v>99</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="91" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="69" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="68" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="94" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="69">
+        <v>1</v>
+      </c>
+      <c r="I12" s="68">
+        <v>1240</v>
+      </c>
+      <c r="J12" s="68"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="68" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="52">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1170</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="92" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" s="92" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" s="93" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="77"/>
+    </row>
+    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>490</v>
+      </c>
+      <c r="M18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>680</v>
+      </c>
+      <c r="M19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="88" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="89" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="G20" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1990</v>
+      </c>
+      <c r="M20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>620</v>
+      </c>
+      <c r="M21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B25" s="96" t="s">
+        <v>144</v>
+      </c>
+      <c r="C25" s="96" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="97" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" s="98" t="s">
+        <v>147</v>
+      </c>
+      <c r="F25" s="99" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="52" t="s">
+        <v>151</v>
+      </c>
+      <c r="F26" s="91" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Pipette] Transformer 비용 요청 - 2/12 email 발송
</commit_message>
<xml_diff>
--- a/Plasma_Gen_Device cost.xlsx
+++ b/Plasma_Gen_Device cost.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -12,12 +12,12 @@
     <sheet name="MOSFET" sheetId="2" r:id="rId3"/>
     <sheet name="Pipette" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="162">
   <si>
     <t>PN</t>
   </si>
@@ -32,18 +32,18 @@
   </si>
   <si>
     <t>220uF/16V ALUMINUM CAPACITORS 6.3pi</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>MVG16VC220MF80</t>
   </si>
   <si>
     <t>MVG16VC220MF80</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>SAMYOUNG</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Agency</t>
@@ -56,34 +56,34 @@
   </si>
   <si>
     <t>재고</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>디바이스마트</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>SMD E/C 16V 220uF (85℃)/6.3Ø x8mm</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>상품코드</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>ICbanQ</t>
   </si>
   <si>
     <t>ICbanQ</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P002101847 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>220uF 16V 85℃-(6.3X7.7)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>NTD5802N</t>
@@ -111,62 +111,62 @@
   </si>
   <si>
     <t>53261-0471</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Molex</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> P005634281 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P001635537</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>수량</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>53398-0471</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P005634253</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>50058-8000</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P005634322</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>장보고</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>CRIMP TERMINAL 51021용 (1.25mm) AWG 28,30,32</t>
   </si>
   <si>
     <t>CRIMP TERMINAL 51021용 (1.25mm) AWG 28,30,32</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>53261-0371</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm 4-Pin SMD RA 1A HEADER</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm 3-Pin SMD RA 1A HEADER</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P_value</t>
@@ -176,25 +176,25 @@
   </si>
   <si>
     <t>51021-0400</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>구매수량</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm 4-Pin Housing, Female</t>
   </si>
   <si>
     <t>1.25mm 4-Pin Housing, Female</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm 4-Pin SMD Straght 1A HEADER</t>
   </si>
   <si>
     <t>1.25mm 4-Pin SMD Straght 1A HEADER</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Power MOSFET 40V, Single N-Channel, 101A DPAK</t>
@@ -204,358 +204,358 @@
   </si>
   <si>
     <t>Total</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>NTD5802N</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P000740132</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P005634281</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>CTX210609-R</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>TRANSFORMER CCFL 6W 13V 11MA SMD Turn-R:100</t>
   </si>
   <si>
     <t>CTX210607-R</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>CTX210605-R</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P002058985</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P005831162</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P002058197</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P007073878 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>부가세</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>부품 Total</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>NTMFS5C604NL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>NTMFS5C468NL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>40 V, 10.3 m , 37 A, Single N−Channel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>60 V, 1.2 m , 287 A, Single N−Channel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>100 V, 16 m , 42 A, Single N−Channel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>BSC160N10NS3 G</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>infineon</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>BSC160N10NS3 G</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>30 V, 0.9m , 47 A, Single N−Channel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>40 V, 7.8 m , 50 A,Single N−Channel, DPAK</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>NVMFS5C673NL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>60 V, 9.2 m , 50 A, Single N−Channel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P007567159</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P007567011</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">ON Semiconductor </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>NVMFS5C450NL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>40 V, 2.8 m , 110 A, Single N−Channel</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>NVMFS5C450NL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>40V, 2.8mOhm , 110A, Single N−Channel Power MOSFET</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>NVMFS5C450NL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>KEMET</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P007223445</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>CAP TANT 220UF 16V 10% 2917</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P008221708</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>장보고 재고 있음</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>2/5일 구매</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>053048-0410</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm Pitch CON,4-Pin, Dip Right angle_Molex</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> P005634295 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>053048-0310</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm Pitch CON,3-Pin, Dip Right angle_Molex</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>CSS-1300C</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> P000394667 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> P000394663 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>CSS-1310TB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> P006911086 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>CSS-1310MC</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>SDS5050TCU-S-AP-A</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve"> (주)디웰전자 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P002343866</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">5.0x5.0x1.6 size, RGB full coler, SMD파워 3색 LED </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Lite-On Inc</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P008219901</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>ASMT-YTD2-0BB02</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Avago</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P000725384 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>LTST-C19HE1WT</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">LTST-C19FD1WT </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P001586603 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>LED RGB DIFFUSED 0606 SMD - 0.35T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>LED OGB DIFFUSED 0608 SMD - 0.55T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>3 color type LED 6-pin, TOP View, R745mcd, G1600mcd, B380mcd</t>
-    <phoneticPr fontId="26" type="noConversion"/>
+    <phoneticPr fontId="27" type="noConversion"/>
   </si>
   <si>
     <t>3.4x2.8</t>
-    <phoneticPr fontId="26" type="noConversion"/>
+    <phoneticPr fontId="27" type="noConversion"/>
   </si>
   <si>
     <t>2.00mm</t>
-    <phoneticPr fontId="26" type="noConversion"/>
+    <phoneticPr fontId="27" type="noConversion"/>
   </si>
   <si>
     <t>LTSN-N213EGBW</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Lite-On Inc</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>3.0x12.5</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>3.5x12</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>3.5mm</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>CL-SB-13A-1x</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>CL-SB-13B-11T</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P006914254</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>CL-SB-13C-11</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P006913975</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>SP3T slide Switch, SMD Right Angle, key 2x0.6</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>SP3T slide Switch, SMD Right Angle, key 2x1.5</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>SP3T slide Switch, DIP Right Angle, key 2x1.5</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>SP3T slide Switch, DIP Right Angle, key 2x0.6</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>SP3T slide Switch, Straight DIP, key 2x0.6</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>CMS-2314A</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>DP3T slide Switch, SMD J-hook Right Angle, key 4x1.5</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>SP3T slide Switch, SMD J-hook Right Angle, key 2x1.5</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Nidec Copal Electronics Corporation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Nidec Copal Electronics Corporation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>5.4x15</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>P_size</t>
@@ -565,61 +565,101 @@
   </si>
   <si>
     <t>12512WS-02B</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>YEONHO</t>
   </si>
   <si>
     <t>CON 2-pin, Throgh hole  type</t>
-    <phoneticPr fontId="26" type="noConversion"/>
+    <phoneticPr fontId="27" type="noConversion"/>
   </si>
   <si>
     <t>5.0x3.6</t>
-    <phoneticPr fontId="26" type="noConversion"/>
+    <phoneticPr fontId="27" type="noConversion"/>
   </si>
   <si>
     <t>4.2mm</t>
   </si>
   <si>
     <t>053048-0210</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>1.25mm Pitch CON,2-Pin, Dip Right angle_Molex</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>4.25x5.5</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Status LED</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Slide Key</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>GAS CON</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>T491D227K016AT</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>재고 없음</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">P007223445 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>2/8일 구매</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>CTX2106</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-R</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>B180212004001</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>주문번호</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>2/12일 구매</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -630,12 +670,20 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1376,160 +1424,160 @@
   </borders>
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
@@ -1546,13 +1594,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1569,7 +1617,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1578,7 +1626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1596,32 +1644,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="21" fillId="33" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="33" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="43" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="33" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="43" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="33" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="43" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="43" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="43" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="52" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="52" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1636,20 +1684,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="52" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="52" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="52" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="41" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1658,10 +1706,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1678,7 +1726,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1688,20 +1736,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1713,16 +1761,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="16" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="16" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="17" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="17" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="17" xfId="43" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="17" xfId="43" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1735,13 +1783,13 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="43" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="43" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="43" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1754,31 +1802,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2008,7 +2059,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2043,7 +2094,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2252,10 +2303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M47"/>
+  <dimension ref="B2:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C14"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2305,13 +2356,13 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="109" t="s">
+      <c r="B4" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="108" t="s">
+      <c r="D4" s="109" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -2339,9 +2390,9 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="109"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
+      <c r="B5" s="114"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="109"/>
       <c r="E5" s="8" t="s">
         <v>16</v>
       </c>
@@ -2538,13 +2589,13 @@
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="109" t="s">
+      <c r="B12" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="108" t="s">
+      <c r="C12" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="108" t="s">
+      <c r="D12" s="109" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="31" t="s">
@@ -2569,9 +2620,9 @@
       </c>
     </row>
     <row r="13" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="109"/>
-      <c r="C13" s="108"/>
-      <c r="D13" s="108"/>
+      <c r="B13" s="114"/>
+      <c r="C13" s="109"/>
+      <c r="D13" s="109"/>
       <c r="E13" s="8" t="s">
         <v>15</v>
       </c>
@@ -2594,9 +2645,9 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="109"/>
-      <c r="C14" s="108"/>
-      <c r="D14" s="108"/>
+      <c r="B14" s="114"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
       <c r="E14" s="8" t="s">
         <v>12</v>
       </c>
@@ -2728,13 +2779,13 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="111" t="s">
+      <c r="B20" s="110" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="108" t="s">
+      <c r="C20" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="110" t="s">
+      <c r="D20" s="108" t="s">
         <v>41</v>
       </c>
       <c r="E20" s="8" t="s">
@@ -2761,9 +2812,9 @@
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="111"/>
-      <c r="C21" s="108"/>
-      <c r="D21" s="110"/>
+      <c r="B21" s="110"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="108"/>
       <c r="E21" s="8" t="s">
         <v>15</v>
       </c>
@@ -2790,13 +2841,13 @@
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="111" t="s">
+      <c r="B22" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="110" t="s">
+      <c r="D22" s="108" t="s">
         <v>40</v>
       </c>
       <c r="E22" s="8" t="s">
@@ -2819,9 +2870,9 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="114"/>
-      <c r="C23" s="113"/>
-      <c r="D23" s="112"/>
+      <c r="B23" s="113"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="111"/>
       <c r="E23" s="10" t="s">
         <v>15</v>
       </c>
@@ -3266,33 +3317,35 @@
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B43" s="34" t="s">
+      <c r="B43" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="36">
+      <c r="C43" s="96">
         <v>1</v>
       </c>
-      <c r="D43" s="48" t="s">
+      <c r="D43" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="48" t="s">
+      <c r="E43" s="95" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="36">
+      <c r="F43" s="96">
         <v>1</v>
       </c>
-      <c r="G43" s="22">
+      <c r="G43" s="97">
         <v>11090</v>
       </c>
-      <c r="H43" s="22">
+      <c r="H43" s="97">
         <v>2</v>
       </c>
-      <c r="I43" s="56">
+      <c r="I43" s="98">
         <f t="shared" si="4"/>
         <v>22180</v>
       </c>
-      <c r="J43" s="33"/>
-      <c r="K43" s="53" t="s">
+      <c r="J43" s="95" t="s">
+        <v>155</v>
+      </c>
+      <c r="K43" s="99" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3348,22 +3401,143 @@
         <v>65098</v>
       </c>
     </row>
+    <row r="51" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="C52" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="H52" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="I52" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="J52" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="K52" s="47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B53" s="117" t="s">
+        <v>158</v>
+      </c>
+      <c r="C53" s="102">
+        <v>1</v>
+      </c>
+      <c r="D53" s="103" t="s">
+        <v>51</v>
+      </c>
+      <c r="E53" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" s="26">
+        <v>2</v>
+      </c>
+      <c r="G53" s="35">
+        <v>13200</v>
+      </c>
+      <c r="H53" s="35">
+        <v>4</v>
+      </c>
+      <c r="I53" s="104">
+        <f t="shared" ref="I53" si="5">G53*H53</f>
+        <v>52800</v>
+      </c>
+      <c r="J53" s="49"/>
+      <c r="K53" s="51" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="I54" s="24">
+        <f>SUM(I53:I53)</f>
+        <v>52800</v>
+      </c>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="I55" s="64">
+        <f>I54*0.1</f>
+        <v>5280</v>
+      </c>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="I56" s="65">
+        <f>I54+I55</f>
+        <v>58080</v>
+      </c>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B12:B14"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B12:B14"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -3445,7 +3619,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3826,7 +4000,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4289,7 +4463,7 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="D7:D8"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Transformer] 부품 재고 Update
</commit_message>
<xml_diff>
--- a/Plasma_Gen_Device cost.xlsx
+++ b/Plasma_Gen_Device cost.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="156">
   <si>
     <t>PN</t>
   </si>
@@ -82,10 +82,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>220uF 16V 85℃-(6.3X7.7)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>NTD5802N</t>
   </si>
   <si>
@@ -107,9 +103,6 @@
     <t>CTX210607-R</t>
   </si>
   <si>
-    <t>TRANSFORMER CCFL 6W 15V 11MA SMD Turn-R:86</t>
-  </si>
-  <si>
     <t>53261-0471</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -118,14 +111,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> P005634281 </t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>P001635537</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>수량</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -134,22 +119,10 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>P005634253</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>50058-8000</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>P005634322</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>장보고</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>CRIMP TERMINAL 51021용 (1.25mm) AWG 28,30,32</t>
   </si>
   <si>
@@ -224,10 +197,6 @@
   </si>
   <si>
     <t>TRANSFORMER CCFL 6W 13V 11MA SMD Turn-R:100</t>
-  </si>
-  <si>
-    <t>CTX210607-R</t>
-    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>CTX210605-R</t>
@@ -659,6 +628,14 @@
   </si>
   <si>
     <t>2/12일 구매</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>재고-2/24</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매수량</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1114,7 +1091,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1429,6 +1406,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1585,7 +1601,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
@@ -1597,11 +1613,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1613,9 +1624,6 @@
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="34" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1706,12 +1714,6 @@
     <xf numFmtId="41" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="176" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1722,9 +1724,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1819,30 +1818,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="24" fillId="34" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="34" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="34" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="34" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="43" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="53">
     <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2070,7 +2106,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2105,7 +2141,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2314,10 +2350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M56"/>
+  <dimension ref="B2:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2329,1224 +2365,1151 @@
     <col min="8" max="8" width="9" style="1"/>
     <col min="9" max="9" width="10.875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="2" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="14" t="s">
+      <c r="H3" s="116" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="116" t="s">
+        <v>155</v>
+      </c>
+      <c r="J3" s="116" t="s">
+        <v>154</v>
+      </c>
+      <c r="K3" s="117" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="118" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="119" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="119" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="45">
         <v>10</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="110" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="109" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="109" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="G4" s="31">
+        <v>90</v>
+      </c>
+      <c r="H4" s="31">
         <v>10</v>
       </c>
-      <c r="G4" s="22">
-        <v>90</v>
-      </c>
-      <c r="H4" s="22">
-        <v>10</v>
-      </c>
-      <c r="I4" s="22">
-        <f>H4*G4</f>
-        <v>900</v>
-      </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="12">
-        <v>4253</v>
+      <c r="I4" s="31">
+        <v>50</v>
+      </c>
+      <c r="J4" s="124">
+        <v>46</v>
+      </c>
+      <c r="K4" s="47" t="s">
+        <v>17</v>
       </c>
       <c r="L4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="110"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="8" t="s">
+    <row r="5" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="103" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="102" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="102" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="44">
+        <v>5</v>
+      </c>
+      <c r="G5" s="18">
+        <v>2280</v>
+      </c>
+      <c r="H5" s="18">
+        <v>10</v>
+      </c>
+      <c r="I5" s="18">
+        <v>10</v>
+      </c>
+      <c r="J5" s="125">
+        <v>3</v>
+      </c>
+      <c r="K5" s="49" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="44">
+        <v>1</v>
+      </c>
+      <c r="G6" s="18">
+        <v>1260</v>
+      </c>
+      <c r="H6" s="18">
+        <v>2</v>
+      </c>
+      <c r="I6" s="18">
+        <v>6</v>
+      </c>
+      <c r="J6" s="125">
+        <v>2</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="66">
+        <v>1</v>
+      </c>
+      <c r="G7" s="120">
+        <v>960</v>
+      </c>
+      <c r="H7" s="18">
+        <v>20</v>
+      </c>
+      <c r="I7" s="18">
+        <v>20</v>
+      </c>
+      <c r="J7" s="125">
+        <v>1</v>
+      </c>
+      <c r="K7" s="49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="44">
+        <v>1</v>
+      </c>
+      <c r="G8" s="18">
+        <v>7100</v>
+      </c>
+      <c r="H8" s="18">
+        <v>2</v>
+      </c>
+      <c r="I8" s="18">
+        <v>2</v>
+      </c>
+      <c r="J8" s="125">
+        <v>0</v>
+      </c>
+      <c r="K8" s="49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="22">
+      <c r="E9" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="44">
+        <v>1</v>
+      </c>
+      <c r="G9" s="18">
+        <v>11090</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18">
+        <v>2</v>
+      </c>
+      <c r="J9" s="125">
+        <v>0</v>
+      </c>
+      <c r="K9" s="49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="121" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="122" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="32">
+        <v>2</v>
+      </c>
+      <c r="G10" s="18">
+        <v>13200</v>
+      </c>
+      <c r="H10" s="18">
+        <v>4</v>
+      </c>
+      <c r="I10" s="123">
+        <v>4</v>
+      </c>
+      <c r="J10" s="125">
+        <v>0</v>
+      </c>
+      <c r="K10" s="49" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="103" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="102" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="102" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="27">
         <v>100</v>
       </c>
-      <c r="H5" s="22">
+      <c r="G11" s="15">
+        <v>130</v>
+      </c>
+      <c r="H11" s="15">
         <v>10</v>
       </c>
-      <c r="I5" s="22">
-        <f>F5*G5</f>
-        <v>5000</v>
-      </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="67" t="s">
-        <v>154</v>
-      </c>
-      <c r="C6" s="66" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="48">
-        <v>5</v>
-      </c>
-      <c r="G6" s="22">
-        <v>2280</v>
-      </c>
-      <c r="H6" s="22">
+      <c r="I11" s="18">
+        <v>100</v>
+      </c>
+      <c r="J11" s="125">
+        <v>89</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="44">
         <v>10</v>
       </c>
-      <c r="I6" s="22">
-        <f>F6*G6</f>
-        <v>11400</v>
-      </c>
-      <c r="J6" s="48"/>
-      <c r="K6" s="53" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="G12" s="18">
+        <v>210</v>
+      </c>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18">
+        <v>30</v>
+      </c>
+      <c r="J12" s="125">
+        <v>14</v>
+      </c>
+      <c r="K12" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="46">
+        <v>100</v>
+      </c>
+      <c r="G13" s="26">
         <v>20</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="H13" s="26">
+        <v>20</v>
+      </c>
+      <c r="I13" s="26">
+        <v>200</v>
+      </c>
+      <c r="J13" s="126">
+        <v>100</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="22">
-        <v>1260</v>
-      </c>
-      <c r="H7" s="22">
+      <c r="D15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="22">
-        <f t="shared" ref="I7:I10" si="0">H7*G7</f>
-        <v>2520</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="12"/>
-    </row>
-    <row r="8" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="70" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="71" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="72" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="72">
-        <v>1</v>
-      </c>
-      <c r="G8" s="73">
-        <v>960</v>
-      </c>
-      <c r="H8" s="22">
-        <v>20</v>
-      </c>
-      <c r="I8" s="22">
-        <f t="shared" si="0"/>
-        <v>19200</v>
-      </c>
-      <c r="J8" s="48"/>
-      <c r="K8" s="53"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="8">
-        <v>1</v>
-      </c>
-      <c r="G9" s="22">
-        <v>7100</v>
-      </c>
-      <c r="H9" s="22">
-        <v>2</v>
-      </c>
-      <c r="I9" s="22">
-        <f t="shared" si="0"/>
-        <v>14200</v>
-      </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="E15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="109" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="8">
-        <v>1</v>
-      </c>
-      <c r="G10" s="22">
-        <v>10080</v>
-      </c>
-      <c r="H10" s="22">
-        <v>2</v>
-      </c>
-      <c r="I10" s="22">
-        <f t="shared" si="0"/>
-        <v>20160</v>
-      </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="12"/>
-    </row>
-    <row r="11" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="8">
-        <v>1</v>
-      </c>
-      <c r="G11" s="22">
-        <v>11090</v>
-      </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="110" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="109" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="109" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="31">
-        <v>100</v>
-      </c>
-      <c r="G12" s="18">
-        <v>130</v>
-      </c>
-      <c r="H12" s="18">
-        <v>10</v>
-      </c>
-      <c r="I12" s="18">
-        <f>F12*G12</f>
-        <v>13000</v>
-      </c>
-      <c r="J12" s="31"/>
-      <c r="K12" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="110"/>
-      <c r="C13" s="109"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1</v>
-      </c>
-      <c r="G13" s="22">
-        <v>1330</v>
-      </c>
-      <c r="H13" s="22">
-        <v>10</v>
-      </c>
-      <c r="I13" s="22">
-        <f t="shared" ref="I13:I14" si="1">H13*G13</f>
-        <v>13300</v>
-      </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="110"/>
-      <c r="C14" s="109"/>
-      <c r="D14" s="109"/>
-      <c r="E14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="8">
-        <v>1</v>
-      </c>
-      <c r="G14" s="22">
-        <v>300</v>
-      </c>
-      <c r="H14" s="22">
-        <v>10</v>
-      </c>
-      <c r="I14" s="22">
-        <f t="shared" si="1"/>
-        <v>3000</v>
-      </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="12">
-        <v>36474</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="11"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="12"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>47</v>
+      <c r="D16" s="107" t="s">
+        <v>34</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="2">
+        <v>100</v>
+      </c>
+      <c r="G16" s="4">
+        <v>90</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="18">
+        <f>F16*G16</f>
+        <v>9000</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="5"/>
+      <c r="L16">
+        <v>650</v>
+      </c>
+      <c r="M16">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="109"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="2">
         <v>10</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G17" s="4">
+        <v>440</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="18">
+        <f>F17*G17</f>
+        <v>4400</v>
+      </c>
+      <c r="J17" s="2"/>
+      <c r="K17" s="5"/>
+      <c r="L17">
+        <f>L16*500</f>
+        <v>325000</v>
+      </c>
+      <c r="M17">
+        <f>M16*10</f>
+        <v>22600</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="108" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="107" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+      <c r="G18" s="4">
+        <v>300</v>
+      </c>
+      <c r="H18" s="18">
+        <v>10</v>
+      </c>
+      <c r="I18" s="18">
+        <f t="shared" ref="I18:I19" si="0">H18*G18</f>
+        <v>3000</v>
+      </c>
+      <c r="J18" s="2"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="112"/>
+      <c r="C19" s="111"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1140</v>
+      </c>
+      <c r="H19" s="26">
+        <v>10</v>
+      </c>
+      <c r="I19" s="26">
+        <f t="shared" si="0"/>
+        <v>11400</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="22" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="71" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="38">
+        <v>1</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="22">
+        <v>50</v>
+      </c>
+      <c r="G24" s="31">
+        <v>100</v>
+      </c>
+      <c r="H24" s="105">
+        <v>50</v>
+      </c>
+      <c r="I24" s="51">
+        <f>G24*H24</f>
+        <v>5000</v>
+      </c>
+      <c r="J24" s="33"/>
+      <c r="K24" s="47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B25" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="39">
+        <v>2</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="32">
+        <v>1</v>
+      </c>
+      <c r="G25" s="18">
+        <v>1260</v>
+      </c>
+      <c r="H25" s="15">
+        <v>6</v>
+      </c>
+      <c r="I25" s="52">
+        <f>G25*H25</f>
+        <v>7560</v>
+      </c>
+      <c r="J25" s="29"/>
+      <c r="K25" s="28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="32">
+        <v>2</v>
+      </c>
+      <c r="D26" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="32">
+        <v>1</v>
+      </c>
+      <c r="G26" s="68">
+        <v>960</v>
+      </c>
+      <c r="H26" s="15">
+        <v>20</v>
+      </c>
+      <c r="I26" s="18">
+        <v>16400</v>
+      </c>
+      <c r="J26" s="29"/>
+      <c r="K26" s="69" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B27" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="39">
+        <v>1</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="32">
+        <v>100</v>
+      </c>
+      <c r="G27" s="18">
+        <v>130</v>
+      </c>
+      <c r="H27" s="15">
+        <v>100</v>
+      </c>
+      <c r="I27" s="52">
+        <f>G27*H27</f>
+        <v>13000</v>
+      </c>
+      <c r="J27" s="29"/>
+      <c r="K27" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="86">
+        <v>1</v>
+      </c>
+      <c r="D28" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="88" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="89">
+        <v>2</v>
+      </c>
+      <c r="G28" s="90">
+        <v>7100</v>
+      </c>
+      <c r="H28" s="90">
+        <v>2</v>
+      </c>
+      <c r="I28" s="91">
+        <f t="shared" ref="I28:I31" si="1">G28*H28</f>
+        <v>14200</v>
+      </c>
+      <c r="J28" s="88" t="s">
+        <v>147</v>
+      </c>
+      <c r="K28" s="92" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="93" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="86">
+        <v>1</v>
+      </c>
+      <c r="D29" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" s="88" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="89">
+        <v>1</v>
+      </c>
+      <c r="G29" s="90">
+        <v>10080</v>
+      </c>
+      <c r="H29" s="90">
+        <v>2</v>
+      </c>
+      <c r="I29" s="91">
+        <f t="shared" si="1"/>
+        <v>20160</v>
+      </c>
+      <c r="J29" s="88" t="s">
+        <v>147</v>
+      </c>
+      <c r="K29" s="92" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="32">
+        <v>1</v>
+      </c>
+      <c r="D30" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="32">
+        <v>1</v>
+      </c>
+      <c r="G30" s="18">
+        <v>11090</v>
+      </c>
+      <c r="H30" s="15">
+        <v>2</v>
+      </c>
+      <c r="I30" s="52">
+        <f t="shared" si="1"/>
+        <v>22180</v>
+      </c>
+      <c r="J30" s="29"/>
+      <c r="K30" s="49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B31" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="39">
+        <v>1</v>
+      </c>
+      <c r="D31" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="32">
+        <v>5</v>
+      </c>
+      <c r="G31" s="18">
         <v>210</v>
       </c>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22">
-        <f>F16*G16</f>
-        <v>2100</v>
-      </c>
-      <c r="J16" s="8"/>
-      <c r="K16" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="10" t="s">
+      <c r="H31" s="15">
+        <v>30</v>
+      </c>
+      <c r="I31" s="52">
+        <f t="shared" si="1"/>
+        <v>6300</v>
+      </c>
+      <c r="J31" s="29"/>
+      <c r="K31" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="40">
+        <v>4</v>
+      </c>
+      <c r="D32" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="23">
+        <v>100</v>
+      </c>
+      <c r="G32" s="26">
+        <v>20</v>
+      </c>
+      <c r="H32" s="104">
+        <v>200</v>
+      </c>
+      <c r="I32" s="55">
+        <f>G32*H32</f>
+        <v>4000</v>
+      </c>
+      <c r="J32" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="K32" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H33" s="57" t="s">
+        <v>57</v>
+      </c>
+      <c r="I33" s="59">
+        <f>SUM(I24:I32)</f>
+        <v>108800</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H34" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="I34" s="60">
+        <f>I33*0.1</f>
+        <v>10880</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="G35" s="14"/>
+      <c r="H35" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="I35" s="61">
+        <f>I33+I34</f>
+        <v>119680</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="71" t="s">
+        <v>149</v>
+      </c>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+    </row>
+    <row r="37" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="I37" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="J37" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="K37" s="43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="94" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="95">
+        <v>1</v>
+      </c>
+      <c r="D38" s="96" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="10">
-        <v>100</v>
-      </c>
-      <c r="G17" s="30">
-        <v>20</v>
-      </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30">
-        <f>F17*G17</f>
-        <v>2000</v>
-      </c>
-      <c r="J17" s="10" t="s">
+      <c r="F38" s="22">
+        <v>2</v>
+      </c>
+      <c r="G38" s="31">
+        <v>7100</v>
+      </c>
+      <c r="H38" s="105">
+        <v>2</v>
+      </c>
+      <c r="I38" s="97">
+        <f t="shared" ref="I38:I40" si="2">G38*H38</f>
+        <v>14200</v>
+      </c>
+      <c r="J38" s="45"/>
+      <c r="K38" s="47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B39" s="93" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="89">
+        <v>1</v>
+      </c>
+      <c r="D39" s="88" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="88" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="89">
+        <v>1</v>
+      </c>
+      <c r="G39" s="90">
+        <v>11090</v>
+      </c>
+      <c r="H39" s="90">
+        <v>2</v>
+      </c>
+      <c r="I39" s="91">
+        <f t="shared" si="2"/>
+        <v>22180</v>
+      </c>
+      <c r="J39" s="88" t="s">
+        <v>147</v>
+      </c>
+      <c r="K39" s="92" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="100" t="s">
+        <v>146</v>
+      </c>
+      <c r="C40" s="98">
+        <v>10</v>
+      </c>
+      <c r="D40" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="99">
+        <v>5</v>
+      </c>
+      <c r="G40" s="6">
+        <v>2280</v>
+      </c>
+      <c r="H40" s="106">
+        <v>10</v>
+      </c>
+      <c r="I40" s="55">
+        <f t="shared" si="2"/>
+        <v>22800</v>
+      </c>
+      <c r="J40" s="3"/>
+      <c r="K40" s="17" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I41" s="20">
+        <f>SUM(I38:I40)</f>
+        <v>59180</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H42" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="I42" s="60">
+        <f>I41*0.1</f>
+        <v>5918</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I43" s="61">
+        <f>I41+I42</f>
+        <v>65098</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="71" t="s">
+        <v>153</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="K17" s="21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="14" t="s">
+      <c r="D48" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G48" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H48" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="I48" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="J48" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="K48" s="43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B49" s="101" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" s="95">
         <v>1</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D49" s="96" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="22">
         <v>2</v>
       </c>
-      <c r="E19" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="112" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="109" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="111" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="2">
-        <v>100</v>
-      </c>
-      <c r="G20" s="4">
-        <v>90</v>
-      </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="22">
-        <f>F20*G20</f>
-        <v>9000</v>
-      </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="5"/>
-      <c r="L20">
-        <v>650</v>
-      </c>
-      <c r="M20">
-        <v>2260</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="112"/>
-      <c r="C21" s="109"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="2">
-        <v>10</v>
-      </c>
-      <c r="G21" s="4">
-        <v>440</v>
-      </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="22">
-        <f>F21*G21</f>
-        <v>4400</v>
-      </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="5"/>
-      <c r="L21">
-        <f>L20*500</f>
-        <v>325000</v>
-      </c>
-      <c r="M21">
-        <f>M20*10</f>
-        <v>22600</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="109" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="111" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" s="4">
-        <v>300</v>
-      </c>
-      <c r="H22" s="22">
-        <v>10</v>
-      </c>
-      <c r="I22" s="22">
-        <f t="shared" ref="I22:I23" si="2">H22*G22</f>
-        <v>3000</v>
-      </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="115"/>
-      <c r="C23" s="114"/>
-      <c r="D23" s="113"/>
-      <c r="E23" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1</v>
-      </c>
-      <c r="G23" s="6">
-        <v>1140</v>
-      </c>
-      <c r="H23" s="30">
-        <v>10</v>
-      </c>
-      <c r="I23" s="30">
-        <f t="shared" si="2"/>
-        <v>11400</v>
-      </c>
-      <c r="J23" s="3"/>
-      <c r="K23" s="7"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="26" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="78" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="E27" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="I27" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="J27" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="K27" s="47" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="42">
-        <v>1</v>
-      </c>
-      <c r="D28" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="26">
-        <v>50</v>
-      </c>
-      <c r="G28" s="35">
-        <v>100</v>
-      </c>
-      <c r="H28" s="119">
-        <v>50</v>
-      </c>
-      <c r="I28" s="55">
-        <f>G28*H28</f>
-        <v>5000</v>
-      </c>
-      <c r="J28" s="37"/>
-      <c r="K28" s="51" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="43">
-        <v>2</v>
-      </c>
-      <c r="D29" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="36">
-        <v>1</v>
-      </c>
-      <c r="G29" s="22">
-        <v>1260</v>
-      </c>
-      <c r="H29" s="18">
-        <v>6</v>
-      </c>
-      <c r="I29" s="56">
-        <f>G29*H29</f>
-        <v>7560</v>
-      </c>
-      <c r="J29" s="33"/>
-      <c r="K29" s="32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="70" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="36">
-        <v>2</v>
-      </c>
-      <c r="D30" s="71" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="74" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="36">
-        <v>1</v>
-      </c>
-      <c r="G30" s="75">
-        <v>960</v>
-      </c>
-      <c r="H30" s="18">
-        <v>20</v>
-      </c>
-      <c r="I30" s="22">
-        <v>16400</v>
-      </c>
-      <c r="J30" s="33"/>
-      <c r="K30" s="76" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="43">
-        <v>1</v>
-      </c>
-      <c r="D31" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="36">
-        <v>100</v>
-      </c>
-      <c r="G31" s="22">
-        <v>130</v>
-      </c>
-      <c r="H31" s="18">
-        <v>100</v>
-      </c>
-      <c r="I31" s="56">
-        <f>G31*H31</f>
-        <v>13000</v>
-      </c>
-      <c r="J31" s="33"/>
-      <c r="K31" s="32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="92" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="93">
-        <v>1</v>
-      </c>
-      <c r="D32" s="94" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" s="95" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="96">
-        <v>2</v>
-      </c>
-      <c r="G32" s="97">
-        <v>7100</v>
-      </c>
-      <c r="H32" s="97">
-        <v>2</v>
-      </c>
-      <c r="I32" s="98">
-        <f t="shared" ref="I32:I35" si="3">G32*H32</f>
-        <v>14200</v>
-      </c>
-      <c r="J32" s="95" t="s">
-        <v>155</v>
-      </c>
-      <c r="K32" s="99" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="100" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="93">
-        <v>1</v>
-      </c>
-      <c r="D33" s="94" t="s">
-        <v>51</v>
-      </c>
-      <c r="E33" s="95" t="s">
-        <v>15</v>
-      </c>
-      <c r="F33" s="96">
-        <v>1</v>
-      </c>
-      <c r="G33" s="97">
-        <v>10080</v>
-      </c>
-      <c r="H33" s="97">
-        <v>2</v>
-      </c>
-      <c r="I33" s="98">
-        <f t="shared" si="3"/>
-        <v>20160</v>
-      </c>
-      <c r="J33" s="95" t="s">
-        <v>155</v>
-      </c>
-      <c r="K33" s="99" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="36">
-        <v>1</v>
-      </c>
-      <c r="D34" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" s="36">
-        <v>1</v>
-      </c>
-      <c r="G34" s="22">
-        <v>11090</v>
-      </c>
-      <c r="H34" s="18">
-        <v>2</v>
-      </c>
-      <c r="I34" s="56">
-        <f t="shared" si="3"/>
-        <v>22180</v>
-      </c>
-      <c r="J34" s="33"/>
-      <c r="K34" s="53" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B35" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="43">
-        <v>1</v>
-      </c>
-      <c r="D35" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="36">
-        <v>5</v>
-      </c>
-      <c r="G35" s="22">
-        <v>210</v>
-      </c>
-      <c r="H35" s="18">
-        <v>30</v>
-      </c>
-      <c r="I35" s="56">
-        <f t="shared" si="3"/>
-        <v>6300</v>
-      </c>
-      <c r="J35" s="33"/>
-      <c r="K35" s="53" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="44">
+      <c r="G49" s="31">
+        <v>13200</v>
+      </c>
+      <c r="H49" s="31">
         <v>4</v>
       </c>
-      <c r="D36" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="E36" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" s="27">
-        <v>100</v>
-      </c>
-      <c r="G36" s="30">
-        <v>20</v>
-      </c>
-      <c r="H36" s="118">
-        <v>200</v>
-      </c>
-      <c r="I36" s="59">
-        <f>G36*H36</f>
-        <v>4000</v>
-      </c>
-      <c r="J36" s="60" t="s">
-        <v>90</v>
-      </c>
-      <c r="K36" s="21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H37" s="61" t="s">
-        <v>65</v>
-      </c>
-      <c r="I37" s="63">
-        <f>SUM(I28:I36)</f>
-        <v>108800</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H38" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="I38" s="64">
-        <f>I37*0.1</f>
-        <v>10880</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="G39" s="17"/>
-      <c r="H39" s="62" t="s">
-        <v>52</v>
-      </c>
-      <c r="I39" s="65">
-        <f>I37+I38</f>
-        <v>119680</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="78" t="s">
-        <v>157</v>
-      </c>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-    </row>
-    <row r="41" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="E41" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="F41" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="H41" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="I41" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="J41" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="K41" s="47" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B42" s="101" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="102">
-        <v>1</v>
-      </c>
-      <c r="D42" s="103" t="s">
-        <v>51</v>
-      </c>
-      <c r="E42" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" s="26">
-        <v>2</v>
-      </c>
-      <c r="G42" s="35">
-        <v>7100</v>
-      </c>
-      <c r="H42" s="119">
-        <v>2</v>
-      </c>
-      <c r="I42" s="104">
-        <f t="shared" ref="I42:I44" si="4">G42*H42</f>
-        <v>14200</v>
-      </c>
-      <c r="J42" s="49"/>
-      <c r="K42" s="51" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B43" s="100" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="96">
-        <v>1</v>
-      </c>
-      <c r="D43" s="95" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" s="95" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43" s="96">
-        <v>1</v>
-      </c>
-      <c r="G43" s="97">
-        <v>11090</v>
-      </c>
-      <c r="H43" s="97">
-        <v>2</v>
-      </c>
-      <c r="I43" s="98">
-        <f t="shared" si="4"/>
-        <v>22180</v>
-      </c>
-      <c r="J43" s="95" t="s">
-        <v>155</v>
-      </c>
-      <c r="K43" s="99" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="107" t="s">
-        <v>154</v>
-      </c>
-      <c r="C44" s="105">
-        <v>10</v>
-      </c>
-      <c r="D44" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="E44" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="F44" s="106">
-        <v>5</v>
-      </c>
-      <c r="G44" s="6">
-        <v>2280</v>
-      </c>
-      <c r="H44" s="120">
-        <v>10</v>
-      </c>
-      <c r="I44" s="59">
-        <f t="shared" si="4"/>
-        <v>22800</v>
-      </c>
-      <c r="J44" s="3"/>
-      <c r="K44" s="21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="I45" s="24">
-        <f>SUM(I42:I44)</f>
-        <v>59180</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H46" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="I46" s="64">
-        <f>I45*0.1</f>
-        <v>5918</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="I47" s="65">
-        <f>I45+I46</f>
-        <v>65098</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="78" t="s">
-        <v>161</v>
-      </c>
+      <c r="I49" s="97">
+        <f t="shared" ref="I49" si="3">G49*H49</f>
+        <v>52800</v>
+      </c>
+      <c r="J49" s="45"/>
+      <c r="K49" s="47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="I50" s="20">
+        <f>SUM(I49:I49)</f>
+        <v>52800</v>
+      </c>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="I51" s="60">
+        <f>I50*0.1</f>
+        <v>5280</v>
+      </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="2:11" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="C52" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D52" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="E52" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="F52" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="G52" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="H52" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="I52" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="J52" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="K52" s="47" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B53" s="108" t="s">
-        <v>158</v>
-      </c>
-      <c r="C53" s="102">
-        <v>1</v>
-      </c>
-      <c r="D53" s="103" t="s">
-        <v>51</v>
-      </c>
-      <c r="E53" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="F53" s="26">
-        <v>2</v>
-      </c>
-      <c r="G53" s="35">
-        <v>13200</v>
-      </c>
-      <c r="H53" s="35">
-        <v>4</v>
-      </c>
-      <c r="I53" s="104">
-        <f t="shared" ref="I53" si="5">G53*H53</f>
-        <v>52800</v>
-      </c>
-      <c r="J53" s="49"/>
-      <c r="K53" s="51" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="I54" s="24">
-        <f>SUM(I53:I53)</f>
-        <v>52800</v>
-      </c>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="I55" s="64">
-        <f>I54*0.1</f>
-        <v>5280</v>
-      </c>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="I56" s="65">
-        <f>I54+I55</f>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="I52" s="61">
+        <f>I50+I51</f>
         <v>58080</v>
       </c>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B12:B14"/>
+  <mergeCells count="6">
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3595,7 +3558,7 @@
         <f>G6/2</f>
         <v>1.1850000000000001</v>
       </c>
-      <c r="H7" s="77">
+      <c r="H7" s="70">
         <f>SUM(F7:G7)</f>
         <v>3.12</v>
       </c>
@@ -3654,133 +3617,133 @@
   <sheetData>
     <row r="1" spans="2:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>20</v>
+        <v>46</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="48">
+      <c r="F3" s="44">
         <v>1</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="18">
         <v>1260</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>20</v>
+        <v>59</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="52" t="s">
-        <v>72</v>
+        <v>63</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>64</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C8" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="63" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="69" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="27">
         <v>1</v>
       </c>
-      <c r="G8" s="68">
+      <c r="G8" s="62">
         <v>960</v>
       </c>
-      <c r="H8" s="68" t="s">
-        <v>79</v>
+      <c r="H8" s="62" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="48">
+      <c r="F9" s="44">
         <v>1</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="18">
         <v>1050</v>
       </c>
-      <c r="H9" s="54" t="s">
-        <v>78</v>
+      <c r="H9" s="50" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
@@ -4034,57 +3997,57 @@
   <sheetData>
     <row r="2" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="87" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="87" t="s">
-        <v>142</v>
-      </c>
-      <c r="G3" s="14" t="s">
+      <c r="E3" s="80" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="80" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="14" t="s">
+      <c r="J3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>28</v>
+        <v>84</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="83" t="s">
-        <v>124</v>
-      </c>
-      <c r="G4" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H4">
@@ -4094,20 +4057,20 @@
         <v>130</v>
       </c>
       <c r="M4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" s="83" t="s">
-        <v>124</v>
-      </c>
-      <c r="G5" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H5">
@@ -4119,26 +4082,26 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="116" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="116" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" s="117" t="s">
+      <c r="B7" s="113" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="113" t="s">
         <v>130</v>
       </c>
+      <c r="D7" s="114" t="s">
+        <v>122</v>
+      </c>
       <c r="E7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F7" s="82" t="s">
-        <v>119</v>
-      </c>
-      <c r="G7" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H7">
@@ -4148,20 +4111,20 @@
         <v>450</v>
       </c>
       <c r="M7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="116"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="117"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="113"/>
+      <c r="D8" s="114"/>
       <c r="E8" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F8" s="82" t="s">
-        <v>119</v>
-      </c>
-      <c r="G8" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="1">
@@ -4171,26 +4134,26 @@
         <v>790</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F9" s="82" t="s">
-        <v>119</v>
-      </c>
-      <c r="G9" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="1">
@@ -4200,140 +4163,140 @@
         <v>700</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" s="52" t="s">
-        <v>137</v>
+        <v>131</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>129</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="76" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="63" t="s">
         <v>123</v>
       </c>
-      <c r="F11" s="83" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="68" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="68" t="s">
-        <v>139</v>
-      </c>
-      <c r="D12" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" s="68" t="s">
-        <v>123</v>
-      </c>
-      <c r="F12" s="86" t="s">
-        <v>124</v>
-      </c>
-      <c r="G12" s="31" t="s">
+      <c r="E12" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="79" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="69">
+      <c r="H12" s="63">
         <v>1</v>
       </c>
-      <c r="I12" s="68">
+      <c r="I12" s="62">
         <v>1240</v>
       </c>
-      <c r="J12" s="68"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="68" t="s">
-        <v>127</v>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="62" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D13" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>124</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F13" s="83" t="s">
-        <v>124</v>
-      </c>
-      <c r="G13" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="76" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="52">
+      <c r="H13" s="48">
         <v>1</v>
       </c>
       <c r="I13" s="1">
         <v>1170</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="77" t="s">
-        <v>135</v>
+      <c r="B14" s="70" t="s">
+        <v>127</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D14" s="84" t="s">
-        <v>136</v>
-      </c>
-      <c r="E14" s="84" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14" s="85" t="s">
-        <v>124</v>
-      </c>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="77"/>
-      <c r="L14" s="77"/>
-      <c r="M14" s="77"/>
+        <v>131</v>
+      </c>
+      <c r="D14" s="77" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" s="77" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" s="78" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="70"/>
+      <c r="M14" s="70"/>
     </row>
     <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
-      </c>
-      <c r="G18" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H18">
@@ -4343,20 +4306,20 @@
         <v>490</v>
       </c>
       <c r="M18" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" t="s">
         <v>107</v>
       </c>
-      <c r="D19" t="s">
-        <v>115</v>
-      </c>
-      <c r="G19" s="48" t="s">
+      <c r="G19" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H19">
@@ -4366,26 +4329,26 @@
         <v>680</v>
       </c>
       <c r="M19" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="80" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="81" t="s">
-        <v>118</v>
-      </c>
-      <c r="F20" s="82" t="s">
-        <v>119</v>
-      </c>
-      <c r="G20" s="48" t="s">
+      <c r="F20" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H20">
@@ -4395,20 +4358,20 @@
         <v>1990</v>
       </c>
       <c r="M20" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G21" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="G21" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H21">
@@ -4418,54 +4381,54 @@
         <v>620</v>
       </c>
       <c r="M21" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="88" t="s">
-        <v>143</v>
-      </c>
-      <c r="C25" s="88" t="s">
-        <v>144</v>
-      </c>
-      <c r="D25" s="89" t="s">
-        <v>145</v>
-      </c>
-      <c r="E25" s="90" t="s">
-        <v>146</v>
-      </c>
-      <c r="F25" s="91" t="s">
-        <v>147</v>
+      <c r="B25" s="81" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="81" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" s="82" t="s">
+        <v>137</v>
+      </c>
+      <c r="E25" s="83" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="84" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C26" s="48" t="s">
-        <v>28</v>
+        <v>140</v>
+      </c>
+      <c r="C26" s="44" t="s">
+        <v>26</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E26" s="52" t="s">
-        <v>150</v>
-      </c>
-      <c r="F26" s="83" t="s">
-        <v>124</v>
+        <v>141</v>
+      </c>
+      <c r="E26" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="F26" s="76" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>